<commit_message>
Corrige planilha de exemplo
</commit_message>
<xml_diff>
--- a/contrib/excep/Excepcionalidade PA EXEMPLO 2023.xlsx
+++ b/contrib/excep/Excepcionalidade PA EXEMPLO 2023.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danilo\dev\python\patic\contrib\excep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\saeb\planejamento-de-tic\contrib\excep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28A4C70-0869-433F-9851-F2D9DCAFC94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD5B883-4756-413B-B29A-45AE5ECE6BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Execução" sheetId="1" r:id="rId1"/>
+    <sheet name="Excepcionalidade" sheetId="1" r:id="rId1"/>
     <sheet name="Config" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Execução!$O$8:$P$1001</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Excepcionalidade!$O$8:$P$1001</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>

</xml_diff>

<commit_message>
Insere o órgão na nome da ação quando não há unidade
</commit_message>
<xml_diff>
--- a/contrib/excep/Excepcionalidade PA EXEMPLO 2023.xlsx
+++ b/contrib/excep/Excepcionalidade PA EXEMPLO 2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\saeb\planejamento-de-tic\contrib\excep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD5B883-4756-413B-B29A-45AE5ECE6BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB878900-4E8E-4CD2-854B-30F002592658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="249">
   <si>
     <t>Execução Plano de Aquisição de TIC</t>
   </si>
@@ -876,6 +876,9 @@
   </si>
   <si>
     <t>Aquisição de roteadores</t>
+  </si>
+  <si>
+    <t>DG</t>
   </si>
 </sst>
 </file>
@@ -2295,7 +2298,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:B4"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2582,7 +2585,9 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
+      <c r="A10" s="38" t="s">
+        <v>248</v>
+      </c>
       <c r="B10" s="38" t="s">
         <v>247</v>
       </c>

</xml_diff>